<commit_message>
Cleaned up main/data input
</commit_message>
<xml_diff>
--- a/Data/Skyhawk_Attributes2.xlsx
+++ b/Data/Skyhawk_Attributes2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Python_Practice\Skyhawk_Modeling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CB2E97-5575-4368-BC2B-A99B26686521}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43BFF77-52FB-4AA1-BB70-FDAA32FB0937}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9156" yWindow="2400" windowWidth="12096" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
+    <workbookView xWindow="9504" yWindow="2748" windowWidth="12096" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -533,13 +533,13 @@
         <v>-0.25</v>
       </c>
       <c r="L2">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="M2">
         <v>0.04</v>
       </c>
       <c r="N2">
-        <v>0.1</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="O2">
         <v>2.5000000000000001E-2</v>

</xml_diff>